<commit_message>
Added some info no code changes
</commit_message>
<xml_diff>
--- a/McKinnon TTLs.xlsx
+++ b/McKinnon TTLs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Website</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>adf.ly</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -153,6 +156,11 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$12</c:f>
@@ -241,11 +249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="271917824"/>
-        <c:axId val="170916864"/>
+        <c:axId val="164011392"/>
+        <c:axId val="183952896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="271917824"/>
+        <c:axId val="164011392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -262,13 +270,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
+                  <a:t>Number of Hops</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Hops</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -279,12 +282,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170916864"/>
+        <c:crossAx val="183952896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170916864"/>
+        <c:axId val="183952896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,13 +305,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time</a:t>
+                  <a:t>Time to Found (sec)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> to Found (sec)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -319,7 +317,367 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="271917824"/>
+        <c:crossAx val="164011392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Distance vs Time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12215</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12771</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.4292999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.095199999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3611000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.291699999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4275000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3894000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6286000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5832999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2140000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5069999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="5204992"/>
+        <c:axId val="5203456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="5204992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="5203456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="5203456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="5204992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Distance vs Hops</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12215</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12771</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12785</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="7467776"/>
+        <c:axId val="7465984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="7467776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="7465984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="7465984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="7467776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -345,16 +703,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -368,6 +726,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -663,15 +1081,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -681,8 +1099,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -692,8 +1113,11 @@
       <c r="C3">
         <v>4.4292999999999996</v>
       </c>
+      <c r="D3">
+        <v>15253</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -703,8 +1127,11 @@
       <c r="C4">
         <v>37.095199999999998</v>
       </c>
+      <c r="D4">
+        <v>12215</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -714,8 +1141,11 @@
       <c r="C5">
         <v>9.3611000000000004</v>
       </c>
+      <c r="D5">
+        <v>12785</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -725,8 +1155,11 @@
       <c r="C6">
         <v>27.291699999999999</v>
       </c>
+      <c r="D6">
+        <v>12785</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -736,8 +1169,11 @@
       <c r="C7">
         <v>4.4275000000000002</v>
       </c>
+      <c r="D7">
+        <v>12771</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -747,8 +1183,11 @@
       <c r="C8">
         <v>5.3894000000000002</v>
       </c>
+      <c r="D8">
+        <v>12785</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -758,8 +1197,11 @@
       <c r="C9">
         <v>9.6286000000000005</v>
       </c>
+      <c r="D9">
+        <v>12785</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -769,8 +1211,11 @@
       <c r="C10">
         <v>2.5832999999999999</v>
       </c>
+      <c r="D10">
+        <v>12011</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -780,8 +1225,11 @@
       <c r="C11">
         <v>5.2140000000000004</v>
       </c>
+      <c r="D11">
+        <v>12785</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -790,6 +1238,9 @@
       </c>
       <c r="C12">
         <v>1.5069999999999999</v>
+      </c>
+      <c r="D12">
+        <v>5837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>